<commit_message>
code dir structure refactored to make gem
</commit_message>
<xml_diff>
--- a/seeds/master_docs.xlsx
+++ b/seeds/master_docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rufaruqui/GitRepos/pure_ruby/mgtool/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B13C3557-4A86-8B4D-BAC2-C676E7E226BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7E179D-977C-854D-94E4-AE5DBA762822}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="1100" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="broker_user_mappings_updated" sheetId="10" r:id="rId1"/>
@@ -40,6 +40,7 @@
             <sz val="12"/>
             <color theme="1"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>@prajakta@radial-solutions.com.au Please confirm book name with Sean. Please note that the book name must be unique for each Business Owner.
 _Assigned to Prajakta Bhamre_
@@ -64,6 +65,7 @@
             <sz val="12"/>
             <color theme="1"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>@prajakta@radial-solutions.com.au Please confirm book name with Sean. Please note that the book name must be unique for each Business Owner.
 _Assigned to Prajakta Bhamre_
@@ -162,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5888" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5889" uniqueCount="606">
   <si>
     <t>Provider_Name</t>
   </si>
@@ -334,6 +336,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">[Sub-Broker] </t>
     </r>
@@ -342,6 +345,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">2 Books:- MFP - Connective - Run Off; LCA - Connective - Accumulation </t>
     </r>
@@ -350,6 +354,7 @@
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>(Merge Both MFP and LCA files as  one)</t>
     </r>
@@ -489,6 +494,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">[Sub-Broker] </t>
     </r>
@@ -497,6 +503,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">3 Books:- RPG - AFG-Accumulation / Fifth - AFG-Maintenance / Impresario - AFG-Run off </t>
     </r>
@@ -505,6 +512,7 @@
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>(Merge all 3 books as 1)</t>
     </r>
@@ -515,6 +523,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">[Sub-Broker] </t>
     </r>
@@ -523,6 +532,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">3 Books:- RPG - AFG-Accumulation / Fifth - AFG-Maintenance / Impresario - AFG-Run off </t>
     </r>
@@ -531,6 +541,7 @@
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>(Merge all 3 books as 1)</t>
     </r>
@@ -544,6 +555,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">[Sub-Broker] </t>
     </r>
@@ -552,6 +564,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">3 Books:- RPG - AFG-Accumulation / Fifth - AFG-Maintenance / Impresario - AFG-Run off </t>
     </r>
@@ -560,6 +573,7 @@
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>(Merge all 3 books as 1)</t>
     </r>
@@ -630,6 +644,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>[Sub-Broker]</t>
     </r>
@@ -638,6 +653,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">  2 Books:- Infinite - Fast-Run off /Fleurieu-Fast-Accumulation</t>
     </r>
@@ -651,6 +667,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>[Sub-Broker]</t>
     </r>
@@ -659,6 +676,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">  2 Books:- Infinite - Fast-Run off /Fleurieu-Fast-Accumulation</t>
     </r>
@@ -813,6 +831,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>[Sub-Broker]</t>
     </r>
@@ -821,6 +840,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> 2 Books:- NVC - Run off /Norman - Run off</t>
     </r>
@@ -831,6 +851,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>[Sub-Broker]</t>
     </r>
@@ -839,6 +860,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> 2 Books:- NVC - Run off /Norman - Run off</t>
     </r>
@@ -1637,6 +1659,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">[Sub-Broker] </t>
     </r>
@@ -1645,6 +1668,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">2 Books:- MFP - Connective - Run Off; LCA - Connective - Accumulation </t>
     </r>
@@ -1653,6 +1677,7 @@
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>(Merge Both MFP and LCA files as  one)</t>
     </r>
@@ -1663,6 +1688,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">[Sub-Broker] </t>
     </r>
@@ -1671,6 +1697,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">3 Books:- RPG - AFG-Accumulation / Fifth - AFG-Maintenance / Impresario - AFG-Run off </t>
     </r>
@@ -1679,6 +1706,7 @@
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>(Merge all 3 books as 1)</t>
     </r>
@@ -1701,6 +1729,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">[Sub-Broker] </t>
     </r>
@@ -1709,6 +1738,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">2 Books:- MFP - Connective - Run Off; LCA - Connective - Accumulation </t>
     </r>
@@ -1717,6 +1747,7 @@
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>(Merge Both MFP and LCA files as  one)</t>
     </r>
@@ -1727,6 +1758,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">[Sub-Broker] </t>
     </r>
@@ -1735,6 +1767,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">3 Books:- RPG - AFG-Accumulation / Fifth - AFG-Maintenance / Impresario - AFG-Run off </t>
     </r>
@@ -1743,6 +1776,7 @@
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>(Merge all 3 books as 1)</t>
     </r>
@@ -2243,16 +2277,19 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2263,21 +2300,25 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2449,7 +2490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2531,6 +2572,8 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2750,7 +2793,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -19756,7 +19799,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC1001"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -19884,7 +19929,7 @@
       <c r="AB2" s="14"/>
       <c r="AC2" s="14"/>
     </row>
-    <row r="3" spans="1:29" ht="31.5" customHeight="1">
+    <row r="3" spans="1:29" ht="19" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -23482,7 +23527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB953"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -24756,10 +24801,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBC6569-6398-134B-A372-131CED862864}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView showGridLines="0" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -24770,7 +24815,7 @@
     <col min="4" max="4" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="39" customFormat="1">
+    <row r="1" spans="1:9" s="39" customFormat="1">
       <c r="A1" s="37" t="s">
         <v>449</v>
       </c>
@@ -24784,22 +24829,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:9">
       <c r="A2" s="35">
         <v>46</v>
       </c>
       <c r="B2" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="51" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="str">
-        <f>LOOKUP(B2,Broker_List!D2:'Broker_List'!D122)</f>
-        <v>2020 Home Loans</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <f>LOOKUP(Broker_List!B2,Broker_List!D2:'Broker_List'!D122)</f>
+        <v>Louisa Sanghera</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="35">
         <v>45</v>
       </c>
@@ -24814,7 +24859,7 @@
         <v>A2B</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:9">
       <c r="A4" s="35">
         <v>37</v>
       </c>
@@ -24829,7 +24874,7 @@
         <v>Akorin</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:9">
       <c r="A5" s="35">
         <v>7</v>
       </c>
@@ -24844,7 +24889,7 @@
         <v>Akorin</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:9">
       <c r="A6" s="35">
         <v>58</v>
       </c>
@@ -24859,7 +24904,7 @@
         <v>Akorin</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:9">
       <c r="A7" s="35">
         <v>6</v>
       </c>
@@ -24874,7 +24919,7 @@
         <v>Akorin</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:9">
       <c r="A8" s="35">
         <v>21</v>
       </c>
@@ -24889,11 +24934,11 @@
         <v>Akorin</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:9">
       <c r="A9" s="35">
         <v>44</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="51" t="s">
         <v>454</v>
       </c>
       <c r="C9" s="34" t="s">
@@ -24904,7 +24949,7 @@
         <v>Akorin</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:9">
       <c r="A10" s="35">
         <v>23</v>
       </c>
@@ -24919,7 +24964,7 @@
         <v>AUS Visage</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:9">
       <c r="A11" s="35">
         <v>73</v>
       </c>
@@ -24934,7 +24979,7 @@
         <v>AUS Visage</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:9">
       <c r="A12" s="35">
         <v>72</v>
       </c>
@@ -24949,7 +24994,7 @@
         <v>AUS Visage</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:9">
       <c r="A13" s="35">
         <v>52</v>
       </c>
@@ -24964,7 +25009,7 @@
         <v>AUS Visage</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:9">
       <c r="A14" s="35">
         <v>26</v>
       </c>
@@ -24979,7 +25024,7 @@
         <v>BPJ Finance</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:9">
       <c r="A15" s="35">
         <v>11</v>
       </c>
@@ -24993,8 +25038,11 @@
         <f>LOOKUP(B15,Broker_List!D2:'Broker_List'!D135)</f>
         <v>BPJ Finance</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="I15" s="52" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="35">
         <v>51</v>
       </c>
@@ -25906,8 +25954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E611F512-BE1C-6744-810D-F56ECE5C859D}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -26422,7 +26470,7 @@
       <c r="A37" s="35">
         <v>42</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="51" t="s">
         <v>472</v>
       </c>
       <c r="C37" s="34" t="s">
@@ -26450,10 +26498,10 @@
       <c r="A39" s="35">
         <v>44</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="51" t="s">
         <v>454</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="51" t="s">
         <v>454</v>
       </c>
       <c r="E39" s="16" t="s">

</xml_diff>

<commit_message>
connective tc type refactor
</commit_message>
<xml_diff>
--- a/seeds/master_docs.xlsx
+++ b/seeds/master_docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rufaruqui/GitRepos/pure_ruby/mgtool/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7E179D-977C-854D-94E4-AE5DBA762822}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62955EDA-3148-0F40-95B7-67197E6536A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="broker_user_mappings_updated" sheetId="10" r:id="rId1"/>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5889" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5895" uniqueCount="613">
   <si>
     <t>Provider_Name</t>
   </si>
@@ -2260,6 +2260,27 @@
   </si>
   <si>
     <t>dump</t>
+  </si>
+  <si>
+    <t>Fort Knox</t>
+  </si>
+  <si>
+    <t>Harbinger-Odyssey</t>
+  </si>
+  <si>
+    <t>The Brokerage</t>
+  </si>
+  <si>
+    <t>Fine Line Finance</t>
+  </si>
+  <si>
+    <t>Malvern Star</t>
+  </si>
+  <si>
+    <t>Pegasus</t>
+  </si>
+  <si>
+    <t>Mortgage Corp</t>
   </si>
 </sst>
 </file>
@@ -2391,7 +2412,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -2486,11 +2507,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2574,6 +2606,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2791,22 +2826,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE8D9EB-E3C8-2048-AB21-258AF9353EC4}">
   <dimension ref="A1:AI1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="5" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="30.7109375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="29.28515625" customWidth="1"/>
     <col min="7" max="7" width="35.42578125" customWidth="1"/>
     <col min="8" max="8" width="23.28515625" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
     <col min="11" max="11" width="24.28515625" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="20.28515625" customWidth="1"/>
     <col min="14" max="14" width="23.140625" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="23.140625" customWidth="1"/>
@@ -2892,7 +2927,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f>LOOKUP(F2, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F2, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>46</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -2962,7 +2997,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f>LOOKUP(F3, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F3, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>45</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -3032,7 +3067,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <f>LOOKUP(F4, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F4, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>45</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -3102,7 +3137,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <f>LOOKUP(F5, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F5, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>37</v>
       </c>
       <c r="C5" s="16" t="s">
@@ -3172,7 +3207,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <f>LOOKUP(F6, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F6, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>23</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -3380,7 +3415,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <f>LOOKUP(F9, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F9, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>51</v>
       </c>
       <c r="C9" s="16" t="s">
@@ -3450,7 +3485,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <f>LOOKUP(F10, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F10, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>41</v>
       </c>
       <c r="C10" s="16" t="s">
@@ -3520,7 +3555,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <f>LOOKUP(F11, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F11, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>80</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -3590,7 +3625,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <f>LOOKUP(F12, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F12, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>72</v>
       </c>
       <c r="C12" s="16" t="s">
@@ -3660,7 +3695,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <f>LOOKUP(F13, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F13, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>74</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -3730,7 +3765,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <f>LOOKUP(F14, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F14, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>71</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -3800,7 +3835,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <f>LOOKUP(F15, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F15, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>71</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -3870,7 +3905,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <f>LOOKUP(F16, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F16, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>71</v>
       </c>
       <c r="C16" s="16" t="s">
@@ -3940,7 +3975,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <f>LOOKUP(F17, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F17,mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>75</v>
       </c>
       <c r="C17" s="16" t="s">
@@ -4010,7 +4045,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <f>LOOKUP(F18, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F18, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>29</v>
       </c>
       <c r="C18" s="16" t="s">
@@ -4080,7 +4115,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <f>LOOKUP(F19, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F19, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>47</v>
       </c>
       <c r="C19" s="16" t="s">
@@ -4150,7 +4185,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <f>LOOKUP(F20, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F20, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>47</v>
       </c>
       <c r="C20" s="16" t="s">
@@ -4220,7 +4255,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <f>LOOKUP(F21, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F21, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>33</v>
       </c>
       <c r="C21" s="16" t="s">
@@ -4290,7 +4325,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <f>LOOKUP(F22, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F22, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>76</v>
       </c>
       <c r="C22" s="16" t="s">
@@ -4360,7 +4395,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <f>LOOKUP(F23, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F23, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>53</v>
       </c>
       <c r="C23" s="16" t="s">
@@ -4430,7 +4465,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <f>LOOKUP(F24, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F24, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>48</v>
       </c>
       <c r="C24" s="16" t="s">
@@ -4500,7 +4535,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <f>LOOKUP(F25, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F25, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>55</v>
       </c>
       <c r="C25" s="16" t="s">
@@ -4570,7 +4605,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <f>LOOKUP(F26, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F26, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>68</v>
       </c>
       <c r="C26" s="16" t="s">
@@ -4640,7 +4675,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <f>LOOKUP(F27, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F27, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>25</v>
       </c>
       <c r="C27" s="16" t="s">
@@ -4710,7 +4745,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <f>LOOKUP(F28, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F28, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>61</v>
       </c>
       <c r="C28" s="16" t="s">
@@ -4780,7 +4815,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <f>LOOKUP(F29, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F29, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>61</v>
       </c>
       <c r="C29" s="16" t="s">
@@ -4850,7 +4885,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <f>LOOKUP(F30, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F30, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>24</v>
       </c>
       <c r="C30" s="16" t="s">
@@ -4920,7 +4955,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <f>LOOKUP(F31, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F31, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>48</v>
       </c>
       <c r="C31" s="16" t="s">
@@ -4990,7 +5025,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <f>LOOKUP(F32, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F32, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>48</v>
       </c>
       <c r="C32" s="16" t="s">
@@ -5060,7 +5095,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <f>LOOKUP(F33, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F33, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>79</v>
       </c>
       <c r="C33" s="16" t="s">
@@ -5130,7 +5165,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <f>LOOKUP(F34, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F34, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>63</v>
       </c>
       <c r="C34" s="44" t="s">
@@ -5200,7 +5235,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <f>LOOKUP(F35, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F35, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>62</v>
       </c>
       <c r="C35" s="16" t="s">
@@ -5270,7 +5305,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <f>LOOKUP(F36, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F36, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>62</v>
       </c>
       <c r="C36" s="16" t="s">
@@ -5340,7 +5375,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <f>LOOKUP(F37, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F37, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>27</v>
       </c>
       <c r="C37" s="16" t="s">
@@ -5410,7 +5445,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <f>LOOKUP(F38, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F38, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>27</v>
       </c>
       <c r="C38" s="16" t="s">
@@ -5480,7 +5515,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <f>LOOKUP(F39, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F39, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>65</v>
       </c>
       <c r="C39" s="16" t="s">
@@ -5550,7 +5585,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <f>LOOKUP(F40, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F40, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>77</v>
       </c>
       <c r="C40" s="16" t="s">
@@ -5620,7 +5655,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <f>LOOKUP(F41, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F41, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>56</v>
       </c>
       <c r="C41" s="16" t="s">
@@ -5690,7 +5725,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <f>LOOKUP(F42, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F42, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>31</v>
       </c>
       <c r="C42" s="44" t="s">
@@ -5760,7 +5795,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <f>LOOKUP(F43, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F43, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>13</v>
       </c>
       <c r="C43" s="16" t="s">
@@ -5830,7 +5865,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <f>LOOKUP(F44, mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F44, mysql_data!B2:B90,mysql_data!A2:A90)</f>
         <v>19</v>
       </c>
       <c r="C44" s="16" t="s">
@@ -9581,8 +9616,8 @@
   <dimension ref="A1:AG1030"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -15789,7 +15824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD0B769-9839-4243-9592-D5607C6EE336}">
   <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -19799,7 +19834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
@@ -24803,8 +24838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBC6569-6398-134B-A372-131CED862864}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView showGridLines="0" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -25954,8 +25989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E611F512-BE1C-6744-810D-F56ECE5C859D}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -26891,7 +26926,7 @@
         <v>72</v>
       </c>
       <c r="B67" s="34" t="s">
-        <v>82</v>
+        <v>460</v>
       </c>
       <c r="C67" s="34" t="s">
         <v>81</v>
@@ -26904,9 +26939,6 @@
       <c r="A68" s="35">
         <v>73</v>
       </c>
-      <c r="B68" s="34" t="s">
-        <v>460</v>
-      </c>
       <c r="C68" s="34" t="s">
         <v>459</v>
       </c>
@@ -27013,41 +27045,83 @@
       </c>
     </row>
     <row r="76" spans="1:5">
+      <c r="A76" s="53">
+        <v>81</v>
+      </c>
+      <c r="B76" t="s">
+        <v>606</v>
+      </c>
       <c r="E76" s="16" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="77" spans="1:5">
+      <c r="A77" s="53">
+        <v>82</v>
+      </c>
+      <c r="B77" t="s">
+        <v>607</v>
+      </c>
       <c r="E77" s="16" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="78" spans="1:5">
+      <c r="A78" s="53">
+        <v>83</v>
+      </c>
+      <c r="B78" t="s">
+        <v>608</v>
+      </c>
       <c r="E78" s="16" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="79" spans="1:5">
+      <c r="A79" s="53">
+        <v>84</v>
+      </c>
+      <c r="B79" t="s">
+        <v>609</v>
+      </c>
       <c r="E79" s="16" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="80" spans="1:5">
+      <c r="A80" s="53">
+        <v>85</v>
+      </c>
+      <c r="B80" t="s">
+        <v>610</v>
+      </c>
       <c r="E80" s="16" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="81" spans="5:5">
+    <row r="81" spans="1:5">
+      <c r="A81" s="53">
+        <v>86</v>
+      </c>
+      <c r="B81" t="s">
+        <v>611</v>
+      </c>
       <c r="E81" s="16" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="82" spans="5:5">
+    <row r="82" spans="1:5">
+      <c r="A82" s="53">
+        <v>87</v>
+      </c>
+      <c r="B82" t="s">
+        <v>612</v>
+      </c>
       <c r="E82" s="16" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="83" spans="5:5">
+    <row r="83" spans="1:5">
       <c r="E83" s="16" t="s">
         <v>427</v>
       </c>
@@ -28824,7 +28898,7 @@
   <dimension ref="A1:AE83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P83"/>
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -28898,7 +28972,7 @@
         <v>#N/A</v>
       </c>
       <c r="B2">
-        <f>LOOKUP(E2,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F2,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>46</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -28950,7 +29024,7 @@
         <v>#N/A</v>
       </c>
       <c r="B3">
-        <f>LOOKUP(E3,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F3,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>45</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -29002,7 +29076,7 @@
         <v>#N/A</v>
       </c>
       <c r="B4">
-        <f>LOOKUP(E4,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F4,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>45</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -29054,7 +29128,7 @@
         <v>#N/A</v>
       </c>
       <c r="B5">
-        <f>LOOKUP(E5,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F5,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>37</v>
       </c>
       <c r="C5" s="16" t="s">
@@ -29106,7 +29180,7 @@
         <v>#N/A</v>
       </c>
       <c r="B6">
-        <f>LOOKUP(E6,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F6,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>23</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -29158,7 +29232,7 @@
         <v>#N/A</v>
       </c>
       <c r="B7">
-        <f>LOOKUP(E7,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F7,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>26</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -29210,7 +29284,7 @@
         <v>#N/A</v>
       </c>
       <c r="B8">
-        <f>LOOKUP(E8,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F8,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>26</v>
       </c>
       <c r="C8" s="16" t="s">
@@ -29260,7 +29334,7 @@
         <v>#N/A</v>
       </c>
       <c r="B9">
-        <f>LOOKUP(E9,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F9,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>51</v>
       </c>
       <c r="C9" s="16" t="s">
@@ -29312,7 +29386,7 @@
         <v>#N/A</v>
       </c>
       <c r="B10">
-        <f>LOOKUP(E10,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F10,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>41</v>
       </c>
       <c r="C10" s="16" t="s">
@@ -29364,7 +29438,7 @@
         <v>#N/A</v>
       </c>
       <c r="B11">
-        <f>LOOKUP(E11,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F11,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>80</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -29416,8 +29490,8 @@
         <v>#N/A</v>
       </c>
       <c r="B12">
-        <f>LOOKUP(E12,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>67</v>
+        <f>LOOKUP(F12,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>72</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>13</v>
@@ -29468,8 +29542,8 @@
         <v>#N/A</v>
       </c>
       <c r="B13">
-        <f>LOOKUP(E13,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>67</v>
+        <f>LOOKUP(F13,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>74</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>13</v>
@@ -29524,7 +29598,7 @@
         <v>#N/A</v>
       </c>
       <c r="B14">
-        <f>LOOKUP(E14,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F14,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>71</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -29580,7 +29654,7 @@
         <v>#N/A</v>
       </c>
       <c r="B15">
-        <f>LOOKUP(E15,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F15,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>71</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -29632,7 +29706,7 @@
         <v>#N/A</v>
       </c>
       <c r="B16">
-        <f>LOOKUP(E16,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F16,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>71</v>
       </c>
       <c r="C16" s="16" t="s">
@@ -29684,7 +29758,7 @@
         <v>#N/A</v>
       </c>
       <c r="B17">
-        <f>LOOKUP(E17,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F17,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>75</v>
       </c>
       <c r="C17" s="16" t="s">
@@ -29736,7 +29810,7 @@
         <v>#N/A</v>
       </c>
       <c r="B18">
-        <f>LOOKUP(E18,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F18,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>29</v>
       </c>
       <c r="C18" s="16" t="s">
@@ -29792,7 +29866,7 @@
         <v>#N/A</v>
       </c>
       <c r="B19">
-        <f>LOOKUP(E19,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F19,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>47</v>
       </c>
       <c r="C19" s="16" t="s">
@@ -29844,7 +29918,7 @@
         <v>#N/A</v>
       </c>
       <c r="B20">
-        <f>LOOKUP(E20,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F20,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>47</v>
       </c>
       <c r="C20" s="16" t="s">
@@ -29896,8 +29970,8 @@
         <v>#N/A</v>
       </c>
       <c r="B21">
-        <f>LOOKUP(E21,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>19</v>
+        <f>LOOKUP(F21,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>33</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>13</v>
@@ -29948,8 +30022,8 @@
         <v>#N/A</v>
       </c>
       <c r="B22">
-        <f>LOOKUP(E22,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>74</v>
+        <f>LOOKUP(F22,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>76</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>13</v>
@@ -30000,7 +30074,7 @@
         <v>#N/A</v>
       </c>
       <c r="B23">
-        <f>LOOKUP(E23,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F23,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>53</v>
       </c>
       <c r="C23" s="16" t="s">
@@ -30052,7 +30126,7 @@
         <v>#N/A</v>
       </c>
       <c r="B24">
-        <f>LOOKUP(E24,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F24,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>48</v>
       </c>
       <c r="C24" s="16" t="s">
@@ -30104,7 +30178,7 @@
         <v>#N/A</v>
       </c>
       <c r="B25">
-        <f>LOOKUP(E25,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F25,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>55</v>
       </c>
       <c r="C25" s="16" t="s">
@@ -30156,7 +30230,7 @@
         <v>#N/A</v>
       </c>
       <c r="B26">
-        <f>LOOKUP(E26,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F26,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>68</v>
       </c>
       <c r="C26" s="16" t="s">
@@ -30208,7 +30282,7 @@
         <v>#N/A</v>
       </c>
       <c r="B27">
-        <f>LOOKUP(E27,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F27,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>25</v>
       </c>
       <c r="C27" s="16" t="s">
@@ -30260,7 +30334,7 @@
         <v>#N/A</v>
       </c>
       <c r="B28">
-        <f>LOOKUP(E28,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F28,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>61</v>
       </c>
       <c r="C28" s="16" t="s">
@@ -30312,7 +30386,7 @@
         <v>#N/A</v>
       </c>
       <c r="B29">
-        <f>LOOKUP(E29,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F29,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>61</v>
       </c>
       <c r="C29" s="16" t="s">
@@ -30364,7 +30438,7 @@
         <v>#N/A</v>
       </c>
       <c r="B30">
-        <f>LOOKUP(E30,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F30,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>24</v>
       </c>
       <c r="C30" s="16" t="s">
@@ -30416,8 +30490,8 @@
         <v>#N/A</v>
       </c>
       <c r="B31">
-        <f>LOOKUP(E31,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>66</v>
+        <f>LOOKUP(F31,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>48</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>13</v>
@@ -30468,8 +30542,8 @@
         <v>#N/A</v>
       </c>
       <c r="B32">
-        <f>LOOKUP(E32,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>66</v>
+        <f>LOOKUP(F32,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>48</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>13</v>
@@ -30520,7 +30594,7 @@
         <v>#N/A</v>
       </c>
       <c r="B33">
-        <f>LOOKUP(E33,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F33,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>79</v>
       </c>
       <c r="C33" s="16" t="s">
@@ -30572,7 +30646,7 @@
         <v>#N/A</v>
       </c>
       <c r="B34">
-        <f>LOOKUP(E34,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F34,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>63</v>
       </c>
       <c r="C34" s="16" t="s">
@@ -30624,7 +30698,7 @@
         <v>#N/A</v>
       </c>
       <c r="B35">
-        <f>LOOKUP(E35,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F35,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>62</v>
       </c>
       <c r="C35" s="16" t="s">
@@ -30676,7 +30750,7 @@
         <v>#N/A</v>
       </c>
       <c r="B36">
-        <f>LOOKUP(E36,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F36,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>62</v>
       </c>
       <c r="C36" s="16" t="s">
@@ -30728,7 +30802,7 @@
         <v>#N/A</v>
       </c>
       <c r="B37">
-        <f>LOOKUP(E37,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F37,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>27</v>
       </c>
       <c r="C37" s="16" t="s">
@@ -30780,7 +30854,7 @@
         <v>#N/A</v>
       </c>
       <c r="B38">
-        <f>LOOKUP(E38,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F38,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>27</v>
       </c>
       <c r="C38" s="16" t="s">
@@ -30832,7 +30906,7 @@
         <v>#N/A</v>
       </c>
       <c r="B39">
-        <f>LOOKUP(E39,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F39,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>65</v>
       </c>
       <c r="C39" s="16" t="s">
@@ -30884,7 +30958,7 @@
         <v>#N/A</v>
       </c>
       <c r="B40">
-        <f>LOOKUP(E40,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F40,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>77</v>
       </c>
       <c r="C40" s="16" t="s">
@@ -30936,8 +31010,8 @@
         <v>#N/A</v>
       </c>
       <c r="B41">
-        <f>LOOKUP(E41,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>77</v>
+        <f>LOOKUP(F41,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>56</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>13</v>
@@ -30988,7 +31062,7 @@
         <v>#N/A</v>
       </c>
       <c r="B42">
-        <f>LOOKUP(E42,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F42,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>31</v>
       </c>
       <c r="C42" s="16" t="s">
@@ -31040,8 +31114,8 @@
         <v>#N/A</v>
       </c>
       <c r="B43">
-        <f>LOOKUP(E43,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>45</v>
+        <f>LOOKUP(F43,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>13</v>
       </c>
       <c r="C43" s="16" t="s">
         <v>252</v>
@@ -31092,8 +31166,8 @@
         <v>#N/A</v>
       </c>
       <c r="B44">
-        <f>LOOKUP(E44,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>37</v>
+        <f>LOOKUP(F44,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>19</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>252</v>
@@ -31144,7 +31218,7 @@
         <v>#N/A</v>
       </c>
       <c r="B45">
-        <f>LOOKUP(E45,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F45,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>6</v>
       </c>
       <c r="C45" s="16" t="s">
@@ -31196,7 +31270,7 @@
         <v>#N/A</v>
       </c>
       <c r="B46">
-        <f>LOOKUP(E46,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F46,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>6</v>
       </c>
       <c r="C46" s="16" t="s">
@@ -31248,8 +31322,8 @@
         <v>#N/A</v>
       </c>
       <c r="B47">
-        <f>LOOKUP(E47,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>21</v>
+        <f>LOOKUP(F47,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>14</v>
       </c>
       <c r="C47" s="16" t="s">
         <v>252</v>
@@ -31300,8 +31374,8 @@
         <v>#N/A</v>
       </c>
       <c r="B48">
-        <f>LOOKUP(E48,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>21</v>
+        <f>LOOKUP(F48,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>14</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>252</v>
@@ -31352,8 +31426,8 @@
         <v>#N/A</v>
       </c>
       <c r="B49">
-        <f>LOOKUP(E49,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>21</v>
+        <f>LOOKUP(F49,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>14</v>
       </c>
       <c r="C49" s="16" t="s">
         <v>252</v>
@@ -31404,8 +31478,8 @@
         <v>#N/A</v>
       </c>
       <c r="B50">
-        <f>LOOKUP(E50,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>21</v>
+        <f>LOOKUP(F50,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>14</v>
       </c>
       <c r="C50" s="16" t="s">
         <v>252</v>
@@ -31456,8 +31530,8 @@
         <v>#N/A</v>
       </c>
       <c r="B51">
-        <f>LOOKUP(E51,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>21</v>
+        <f>LOOKUP(F51,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>14</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>252</v>
@@ -31508,8 +31582,8 @@
         <v>#N/A</v>
       </c>
       <c r="B52">
-        <f>LOOKUP(E52,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>21</v>
+        <f>LOOKUP(F52,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>14</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>252</v>
@@ -31560,7 +31634,7 @@
         <v>#N/A</v>
       </c>
       <c r="B53">
-        <f>LOOKUP(E53,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F53,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>52</v>
       </c>
       <c r="C53" s="16" t="s">
@@ -31612,8 +31686,8 @@
         <v>#N/A</v>
       </c>
       <c r="B54">
-        <f>LOOKUP(E54,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>51</v>
+        <f>LOOKUP(F54,mysql_data!B2:B75,mysql_data!A3:A76)</f>
+        <v>40</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>252</v>
@@ -31664,8 +31738,8 @@
         <v>#N/A</v>
       </c>
       <c r="B55">
-        <f>LOOKUP(E55,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>51</v>
+        <f>LOOKUP(F55,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>16</v>
       </c>
       <c r="C55" s="16" t="s">
         <v>252</v>
@@ -31716,7 +31790,7 @@
         <v>#N/A</v>
       </c>
       <c r="B56">
-        <f>LOOKUP(E56,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F56,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>70</v>
       </c>
       <c r="C56" s="16" t="s">
@@ -31768,7 +31842,7 @@
         <v>#N/A</v>
       </c>
       <c r="B57">
-        <f>LOOKUP(E57,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F57,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>70</v>
       </c>
       <c r="C57" s="16" t="s">
@@ -31820,8 +31894,8 @@
         <v>#N/A</v>
       </c>
       <c r="B58">
-        <f>LOOKUP(E58,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>70</v>
+        <f>LOOKUP(F58,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>30</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>252</v>
@@ -31872,8 +31946,8 @@
         <v>#N/A</v>
       </c>
       <c r="B59">
-        <f>LOOKUP(E59,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>70</v>
+        <f>LOOKUP(F59,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>30</v>
       </c>
       <c r="C59" s="16" t="s">
         <v>252</v>
@@ -31924,8 +31998,8 @@
         <v>#N/A</v>
       </c>
       <c r="B60">
-        <f>LOOKUP(E60,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>70</v>
+        <f>LOOKUP(F60,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>30</v>
       </c>
       <c r="C60" s="16" t="s">
         <v>252</v>
@@ -31976,8 +32050,8 @@
         <v>#N/A</v>
       </c>
       <c r="B61">
-        <f>LOOKUP(E61,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>67</v>
+        <f>LOOKUP(F61,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>69</v>
       </c>
       <c r="C61" s="16" t="s">
         <v>252</v>
@@ -32028,7 +32102,7 @@
         <v>#N/A</v>
       </c>
       <c r="B62">
-        <f>LOOKUP(E62,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F62,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>67</v>
       </c>
       <c r="C62" s="16" t="s">
@@ -32080,7 +32154,7 @@
         <v>#N/A</v>
       </c>
       <c r="B63">
-        <f>LOOKUP(E63,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F63,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>67</v>
       </c>
       <c r="C63" s="16" t="s">
@@ -32132,8 +32206,8 @@
         <v>#N/A</v>
       </c>
       <c r="B64">
-        <f>LOOKUP(E64,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>38</v>
+        <f>LOOKUP(F64,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>10</v>
       </c>
       <c r="C64" s="16" t="s">
         <v>252</v>
@@ -32184,8 +32258,8 @@
         <v>#N/A</v>
       </c>
       <c r="B65">
-        <f>LOOKUP(E65,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>38</v>
+        <f>LOOKUP(F65,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>10</v>
       </c>
       <c r="C65" s="16" t="s">
         <v>252</v>
@@ -32236,8 +32310,8 @@
         <v>#N/A</v>
       </c>
       <c r="B66">
-        <f>LOOKUP(E66,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>38</v>
+        <f>LOOKUP(F66,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>10</v>
       </c>
       <c r="C66" s="16" t="s">
         <v>252</v>
@@ -32288,8 +32362,8 @@
         <v>#N/A</v>
       </c>
       <c r="B67">
-        <f>LOOKUP(E67,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>38</v>
+        <f>LOOKUP(F67,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>10</v>
       </c>
       <c r="C67" s="16" t="s">
         <v>252</v>
@@ -32340,8 +32414,8 @@
         <v>#N/A</v>
       </c>
       <c r="B68">
-        <f>LOOKUP(E68,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>38</v>
+        <f>LOOKUP(F68,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>10</v>
       </c>
       <c r="C68" s="16" t="s">
         <v>252</v>
@@ -32392,8 +32466,8 @@
         <v>#N/A</v>
       </c>
       <c r="B69">
-        <f>LOOKUP(E69,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>71</v>
+        <f>LOOKUP(F69,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>15</v>
       </c>
       <c r="C69" s="16" t="s">
         <v>252</v>
@@ -32444,7 +32518,7 @@
         <v>#N/A</v>
       </c>
       <c r="B70">
-        <f>LOOKUP(E70,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <f>LOOKUP(F70,mysql_data!B2:B75,mysql_data!A2:A75)</f>
         <v>78</v>
       </c>
       <c r="C70" s="16" t="s">
@@ -32496,8 +32570,8 @@
         <v>#N/A</v>
       </c>
       <c r="B71">
-        <f>LOOKUP(E71,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>29</v>
+        <f>LOOKUP(F71,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>54</v>
       </c>
       <c r="C71" s="16" t="s">
         <v>252</v>
@@ -32548,8 +32622,8 @@
         <v>#N/A</v>
       </c>
       <c r="B72">
-        <f>LOOKUP(E72,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>29</v>
+        <f>LOOKUP(F72,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>2</v>
       </c>
       <c r="C72" s="16" t="s">
         <v>252</v>
@@ -32600,8 +32674,8 @@
         <v>#N/A</v>
       </c>
       <c r="B73">
-        <f>LOOKUP(E73,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>29</v>
+        <f>LOOKUP(F73,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>2</v>
       </c>
       <c r="C73" s="16" t="s">
         <v>252</v>
@@ -32652,8 +32726,8 @@
         <v>#N/A</v>
       </c>
       <c r="B74">
-        <f>LOOKUP(E74,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>29</v>
+        <f>LOOKUP(F74,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>2</v>
       </c>
       <c r="C74" s="16" t="s">
         <v>252</v>
@@ -32704,8 +32778,8 @@
         <v>#N/A</v>
       </c>
       <c r="B75">
-        <f>LOOKUP(E75,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>29</v>
+        <f>LOOKUP(F75,mysql_data!B2:B75,mysql_data!A2:A75)</f>
+        <v>2</v>
       </c>
       <c r="C75" s="16" t="s">
         <v>252</v>
@@ -32756,8 +32830,8 @@
         <v>#N/A</v>
       </c>
       <c r="B76">
-        <f>LOOKUP(E76,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>29</v>
+        <f ca="1">LOOKUP(F76,mysql_data!B2:B90,mysql_data!A3:A76)</f>
+        <v>6</v>
       </c>
       <c r="C76" s="16" t="s">
         <v>252</v>
@@ -32808,8 +32882,8 @@
         <v>#N/A</v>
       </c>
       <c r="B77">
-        <f>LOOKUP(E77,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>54</v>
+        <f ca="1">LOOKUP(F77,mysql_data!B3:B91,mysql_data!A4:A77)</f>
+        <v>58</v>
       </c>
       <c r="C77" s="16" t="s">
         <v>252</v>
@@ -32860,8 +32934,8 @@
         <v>#N/A</v>
       </c>
       <c r="B78">
-        <f>LOOKUP(E78,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>54</v>
+        <f ca="1">LOOKUP(F78,mysql_data!B4:B92,mysql_data!A5:A78)</f>
+        <v>58</v>
       </c>
       <c r="C78" s="16" t="s">
         <v>252</v>
@@ -32912,8 +32986,8 @@
         <v>#N/A</v>
       </c>
       <c r="B79">
-        <f>LOOKUP(E79,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>24</v>
+        <f ca="1">LOOKUP(F79,mysql_data!B5:B93,mysql_data!A6:A79)</f>
+        <v>51</v>
       </c>
       <c r="C79" s="16" t="s">
         <v>252</v>
@@ -32964,8 +33038,8 @@
         <v>#N/A</v>
       </c>
       <c r="B80">
-        <f>LOOKUP(E80,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>63</v>
+        <f ca="1">LOOKUP(F80,mysql_data!B6:B94,mysql_data!A7:A80)</f>
+        <v>12</v>
       </c>
       <c r="C80" s="16" t="s">
         <v>252</v>
@@ -33016,8 +33090,8 @@
         <v>#N/A</v>
       </c>
       <c r="B81">
-        <f>LOOKUP(E81,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>18</v>
+        <f ca="1">LOOKUP(F81,mysql_data!B7:B95,mysql_data!A8:A81)</f>
+        <v>69</v>
       </c>
       <c r="C81" s="16" t="s">
         <v>252</v>
@@ -33068,8 +33142,8 @@
         <v>#N/A</v>
       </c>
       <c r="B82">
-        <f>LOOKUP(E82,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>18</v>
+        <f ca="1">LOOKUP(F82,mysql_data!B8:B96,mysql_data!A9:A82)</f>
+        <v>69</v>
       </c>
       <c r="C82" s="16" t="s">
         <v>252</v>
@@ -33120,8 +33194,8 @@
         <v>#N/A</v>
       </c>
       <c r="B83">
-        <f>LOOKUP(E83,mysql_data!B2:B75,mysql_data!A2:A75)</f>
-        <v>77</v>
+        <f ca="1">LOOKUP(F83,mysql_data!B9:B97,mysql_data!A10:A83)</f>
+        <v>31</v>
       </c>
       <c r="C83" s="16" t="s">
         <v>252</v>

</xml_diff>